<commit_message>
Jerarquias y relaciones recursivas
</commit_message>
<xml_diff>
--- a/Unidad I/ModelosER/PruebasAerolinea.xlsx
+++ b/Unidad I/ModelosER/PruebasAerolinea.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="12495" windowHeight="4320"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="12495" windowHeight="4320"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>AVION</t>
   </si>
@@ -179,12 +179,6 @@
     <t>PILOTO</t>
   </si>
   <si>
-    <t>COPILOTO</t>
-  </si>
-  <si>
-    <t>AREMOSO</t>
-  </si>
-  <si>
     <t>NUMERO_VUELO</t>
   </si>
   <si>
@@ -219,6 +213,105 @@
   </si>
   <si>
     <t>ORDEN</t>
+  </si>
+  <si>
+    <t>MATUSALEN</t>
+  </si>
+  <si>
+    <t>RODRIGO</t>
+  </si>
+  <si>
+    <t>JESUS</t>
+  </si>
+  <si>
+    <t>CODIGO_TRIPULANTE_SUPERIOR</t>
+  </si>
+  <si>
+    <t>PAIS</t>
+  </si>
+  <si>
+    <t>CODIGO_PAIS</t>
+  </si>
+  <si>
+    <t>NOMBRE_PAIS</t>
+  </si>
+  <si>
+    <t>DEPARTAMENTO</t>
+  </si>
+  <si>
+    <t>CODIGO_DEPARTAMENTO</t>
+  </si>
+  <si>
+    <t>NOMBRE_DEPARTAMENTO</t>
+  </si>
+  <si>
+    <t>MUNICIPIO</t>
+  </si>
+  <si>
+    <t>CODIGO_MUNICIPIO</t>
+  </si>
+  <si>
+    <t>NOMBRE_MUNICIPIO</t>
+  </si>
+  <si>
+    <t>GUATEMALA</t>
+  </si>
+  <si>
+    <t>FRANCISCO MORAZAN</t>
+  </si>
+  <si>
+    <t>INTIBUCA</t>
+  </si>
+  <si>
+    <t>LEMPIRA</t>
+  </si>
+  <si>
+    <t>TEGUCIGALPA</t>
+  </si>
+  <si>
+    <t>DISTRITO CENTRAL</t>
+  </si>
+  <si>
+    <t>VALLE DE ANGELES</t>
+  </si>
+  <si>
+    <t>LA ESPERANZA</t>
+  </si>
+  <si>
+    <t>GRACIAS</t>
+  </si>
+  <si>
+    <t>LUGAR</t>
+  </si>
+  <si>
+    <t>LUGAR_PADRE</t>
+  </si>
+  <si>
+    <t>AMERICA</t>
+  </si>
+  <si>
+    <t>CENTRO AMERICA</t>
+  </si>
+  <si>
+    <t>COMAYAGUELA</t>
+  </si>
+  <si>
+    <t>CODIGO_TIPO_LUGAR</t>
+  </si>
+  <si>
+    <t>HORAS_VUELO</t>
+  </si>
+  <si>
+    <t>ESPECIALIZACION</t>
+  </si>
+  <si>
+    <t>CODIGO_TIPO_TRIPULANTE</t>
+  </si>
+  <si>
+    <t>CODIGO_PILOTO</t>
+  </si>
+  <si>
+    <t>EN VOLAR</t>
   </si>
 </sst>
 </file>
@@ -257,7 +350,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -506,11 +599,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -535,6 +639,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,16 +924,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:I80"/>
+  <dimension ref="A6:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -950,7 +1060,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>2</v>
       </c>
@@ -967,10 +1077,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -978,7 +1088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
@@ -996,7 +1106,7 @@
       </c>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>1</v>
       </c>
@@ -1013,7 +1123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
         <v>2</v>
       </c>
@@ -1030,7 +1140,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
         <v>3</v>
       </c>
@@ -1047,7 +1157,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F26" s="7">
         <v>4</v>
       </c>
@@ -1055,12 +1165,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
       <c r="F29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="F30" s="20" t="s">
         <v>22</v>
       </c>
@@ -1068,7 +1190,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <v>40</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="F31" s="5">
         <v>1</v>
       </c>
@@ -1076,7 +1207,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="F32" s="5">
         <v>1</v>
       </c>
@@ -1084,7 +1218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F33" s="5">
         <v>1</v>
       </c>
@@ -1092,7 +1226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="7">
         <v>2</v>
       </c>
@@ -1100,33 +1234,154 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F35" s="18"/>
       <c r="G35" s="19"/>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F36" s="18"/>
       <c r="G36" s="19"/>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
       <c r="F37" s="18"/>
       <c r="G37" s="19"/>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>93</v>
+      </c>
       <c r="F38" s="18"/>
       <c r="G38" s="19"/>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>4</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>5</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="17">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
+        <v>6</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="17">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2</v>
+      </c>
+    </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -1134,10 +1389,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -1145,13 +1397,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" t="s">
-        <v>51</v>
-      </c>
-      <c r="E52" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -1159,301 +1405,560 @@
         <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="F53" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E54" s="1">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1">
-        <v>1</v>
+      <c r="F54" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I54" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E55" s="1">
-        <v>1</v>
-      </c>
       <c r="F55" s="1">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E56" s="1">
-        <v>2</v>
-      </c>
       <c r="F56" s="1">
         <v>1</v>
       </c>
+      <c r="G56" s="1">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="1">
-        <v>2</v>
-      </c>
       <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1">
+        <v>3</v>
+      </c>
+      <c r="I57">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>31</v>
+      <c r="B58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>4</v>
+      </c>
+      <c r="I58">
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="1">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>35</v>
+      <c r="B59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" s="17">
+        <v>1</v>
+      </c>
+      <c r="G59" s="17">
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="17">
+        <v>2</v>
+      </c>
+      <c r="G60" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F62" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F61" s="17">
+        <v>2</v>
+      </c>
+      <c r="G61" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G62" s="23" t="s">
+      <c r="E66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>2</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>3</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H62" t="s">
-        <v>63</v>
-      </c>
-      <c r="I62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F63" s="1">
-        <v>1</v>
-      </c>
-      <c r="G63" s="1">
-        <v>1</v>
-      </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F64" s="1">
-        <v>1</v>
-      </c>
-      <c r="G64" s="1">
-        <v>2</v>
-      </c>
-      <c r="I64">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F65" s="1">
-        <v>1</v>
-      </c>
-      <c r="G65" s="1">
-        <v>3</v>
-      </c>
-      <c r="I65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>42</v>
-      </c>
-      <c r="F66" s="1">
-        <v>1</v>
-      </c>
-      <c r="G66" s="1">
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1">
+        <v>2</v>
+      </c>
+      <c r="E70" s="1">
+        <v>3</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>2</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2</v>
+      </c>
+      <c r="E71" s="1">
         <v>4</v>
       </c>
-      <c r="I66">
+      <c r="F71" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2</v>
+      </c>
+      <c r="E72" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F67" s="17">
-        <v>1</v>
-      </c>
-      <c r="G67" s="17">
+      <c r="F72" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>67</v>
+      </c>
+      <c r="F98" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F99" t="s">
+        <v>55</v>
+      </c>
+      <c r="G99" t="s">
+        <v>56</v>
+      </c>
+      <c r="H99" t="s">
+        <v>86</v>
+      </c>
+      <c r="I99" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="1">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H100" s="4"/>
+      <c r="I100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="1">
+        <v>2</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F101" s="5">
+        <v>2</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H101" s="6">
+        <v>1</v>
+      </c>
+      <c r="I101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="1">
+        <v>3</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F102" s="5">
+        <v>3</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H102" s="6">
+        <v>2</v>
+      </c>
+      <c r="I102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F103" s="5">
+        <v>4</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H103" s="6">
+        <v>2</v>
+      </c>
+      <c r="I103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F104" s="5">
         <v>5</v>
       </c>
-      <c r="I67">
+      <c r="G104" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H104" s="6">
+        <v>2</v>
+      </c>
+      <c r="I104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>70</v>
+      </c>
+      <c r="F105" s="5">
+        <v>6</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H105" s="6">
+        <v>3</v>
+      </c>
+      <c r="I105">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="1">
-        <v>1</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F68" s="17">
-        <v>2</v>
-      </c>
-      <c r="G68" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="1">
-        <v>2</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F69" s="17">
-        <v>2</v>
-      </c>
-      <c r="G69" s="17">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F106" s="5">
+        <v>7</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H106" s="6">
+        <v>3</v>
+      </c>
+      <c r="I106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="1">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D107" s="1">
+        <v>1</v>
+      </c>
+      <c r="F107" s="5">
+        <v>8</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H107" s="6">
+        <v>3</v>
+      </c>
+      <c r="I107" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="1">
+        <v>2</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
+      <c r="F108" s="25">
+        <v>9</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H108" s="26">
+        <v>6</v>
+      </c>
+      <c r="I108" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E74" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="1">
-        <v>1</v>
-      </c>
-      <c r="C75" s="1">
-        <v>1</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="1">
-        <v>2</v>
-      </c>
-      <c r="C76" s="1">
-        <v>1</v>
-      </c>
-      <c r="E76" s="1">
-        <v>1</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="1">
-        <v>3</v>
-      </c>
-      <c r="C77" s="1">
-        <v>1</v>
-      </c>
-      <c r="E77" s="1">
-        <v>2</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="1">
-        <v>1</v>
-      </c>
-      <c r="C78" s="1">
-        <v>2</v>
-      </c>
-      <c r="E78" s="1">
-        <v>3</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="1">
-        <v>2</v>
-      </c>
-      <c r="C79" s="1">
-        <v>2</v>
-      </c>
-      <c r="E79" s="1">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="1">
+        <v>3</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
+      </c>
+      <c r="F109" s="25">
+        <v>10</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H109" s="26">
+        <v>6</v>
+      </c>
+      <c r="I109" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F110" s="25">
+        <v>11</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H110" s="26">
+        <v>7</v>
+      </c>
+      <c r="I110" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F111" s="27">
+        <v>12</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H111" s="28">
+        <v>8</v>
+      </c>
+      <c r="I111" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>73</v>
+      </c>
+      <c r="F112" s="18">
+        <v>13</v>
+      </c>
+      <c r="G112" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H112" s="19">
+        <v>9</v>
+      </c>
+      <c r="I112" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F113" s="18">
+        <v>14</v>
+      </c>
+      <c r="G113" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H113" s="19">
+        <v>9</v>
+      </c>
+      <c r="I113" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="1">
+        <v>1</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="1">
+        <v>2</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="1">
+        <v>3</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D116" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="1">
         <v>4</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="1">
-        <v>3</v>
-      </c>
-      <c r="C80" s="1">
-        <v>2</v>
-      </c>
-      <c r="E80" s="1">
-        <v>5</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>45</v>
+      <c r="C117" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D117" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>